<commit_message>
Add xlwings pro notebook
</commit_message>
<xml_diff>
--- a/notebook/rdp_report.xlsx
+++ b/notebook/rdp_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive_d\Project\Code\xlwings_rdlib_project\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{935DA15A-7507-48C3-BC78-B7CCC4445433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{628560CA-6C98-4240-88AF-3E299BCCAFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="1380" windowWidth="19890" windowHeight="11535" xr2:uid="{AEF1BE34-BB7F-4748-BCB4-5FA47DCEEBBD}"/>
+    <workbookView xWindow="1125" yWindow="1545" windowWidth="22710" windowHeight="13275" xr2:uid="{C1C3D441-6D75-464C-A143-6D2C9D4C856A}"/>
   </bookViews>
   <sheets>
     <sheet name="LSEG.L News Data" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -78,73 +78,70 @@
     <t>sourceCode</t>
   </si>
   <si>
-    <t>ADR Recap: London Stock Exchange continues to outperform Wolters Kluwer</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20231106:nNRAqle9br:0</t>
-  </si>
-  <si>
-    <t>NS:GLOROU</t>
-  </si>
-  <si>
-    <t>Monday November 06, 2023 London Stock Exchange ADR Compendium - A Snapshot as of November 06</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20231106:nNRAqle2r7:0</t>
-  </si>
-  <si>
-    <t>Monday November 06, 2023 London Stock Exchange ADR: How it compares to other IDRs and ADRs</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20231106:nNRAqle2sx:0</t>
-  </si>
-  <si>
-    <t>ADR Recap: London Stock Exchange continues to outperform Macquarie Group</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20231106:nNRAqldlgj:0</t>
-  </si>
-  <si>
-    <t>ADR Recap: London Stock Exchange continues to outperform Hong Kong Exchanges &amp; Clearing</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20231106:nNRAqld38y:0</t>
-  </si>
-  <si>
-    <t>Monthly: London Stock Exchange ADR (LNSTY: $25.46) increases 2% on weak volume in October 2023</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20231106:nNRAqlct8r:0</t>
-  </si>
-  <si>
-    <t>ADR Recap: London Stock Exchange continues to outperform Deutsche Boerse</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20231106:nNRAqlcdv4:0</t>
-  </si>
-  <si>
-    <t>Citigroup Reiterates "Buy" Rating for London Stock Exchange Group (LON:LSEG)</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20231106:nNRAqlbihx:0</t>
-  </si>
-  <si>
-    <t>NS:COMFIN</t>
-  </si>
-  <si>
-    <t>London Stock Exchange Group (LON:LSEG) Stock Rating Reaffirmed by Citigroup</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20231106:nNRAqlbb13:0</t>
-  </si>
-  <si>
-    <t>NS:WATNEW</t>
-  </si>
-  <si>
-    <t>How London Stock Exchange's dividend compares to China Galaxy</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20231106:nNRAqlbeu6:0</t>
+    <t>London Stock Exchange Group continues to underperform Intermediate Capital</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20231107:nNRAqll2kb:0</t>
+  </si>
+  <si>
+    <t>NS:NEWMAR</t>
+  </si>
+  <si>
+    <t>London Stock Exchange Group continues to underperform M&amp;G</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20231107:nNRAqlk82m:0</t>
+  </si>
+  <si>
+    <t>London Stock Exchange Group's Earnings Growth Outperforms Hargreaves Lansdown</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20231107:nNRAqlk7t4:0</t>
+  </si>
+  <si>
+    <t>London Stock Exchange Group (LSEG: GBX8,314.0) - PRE-MARKET CONFIRMATORY BULLISH SIGNAL FROM ITS ADR MARKET Tuesday November 07, 2023 06:11 GMT</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20231107:nNRAqljhxn:0</t>
+  </si>
+  <si>
+    <t>NS:GLOBUL</t>
+  </si>
+  <si>
+    <t>UNITED KINGDOM PRE-MARKET BULLISH STOCK SNIPPETS LONDON STOCK EXCHANGE GROUP (LSEG: GBX8,314.0) Tuesday November 07, 2023 06:11 GMT</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20231107:nNRAqljii0:0</t>
+  </si>
+  <si>
+    <t>London Stock Exchange Group's Earnings Growth Lags 3I Group</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20231107:nNRAqljcyu:0</t>
+  </si>
+  <si>
+    <t>London Stock Exchange Group continues to outperform Schroders</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20231107:nNRAqljd3i:0</t>
+  </si>
+  <si>
+    <t>How London Stock Exchange Group's dividend compares to Intermediate Capital</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20231107:nNRAqljchb:0</t>
+  </si>
+  <si>
+    <t>Hargreaves Lansdown's Earnings Growth Lags London Stock Exchange Group</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20231107:nNRAqlif88:0</t>
+  </si>
+  <si>
+    <t>Close Brothers's Earnings Growth Lags London Stock Exchange Group</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20231107:nNRAqliewr:0</t>
   </si>
 </sst>
 </file>
@@ -252,7 +249,7 @@
         <xdr:cNvPr id="3" name="MyPlot">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F4FF73C-EEDB-EAC3-CDC3-C8DC2A6892FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4395D96-B02A-EB28-DCD7-ED76782AB2C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -583,7 +580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD63981-5CAB-455E-83CB-805B346D9EAC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1486732-1EB2-479B-A8D7-04925134B9E9}">
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -685,26 +682,26 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -712,10 +709,10 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -723,13 +720,13 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -740,15 +737,15 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -760,10 +757,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7520AD08-1635-4384-B4FB-F87CD556085A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91377A17-0F5E-4FDC-8289-C00E7D725E16}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Update images Update dataset
</commit_message>
<xml_diff>
--- a/notebook/rdp_report.xlsx
+++ b/notebook/rdp_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive_d\Project\Code\xlwings_rdlib_project\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B78516EB-2CAE-482E-925D-CE38664C2149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0103D0F-209E-4822-BA9B-8DBB29F8C0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D15E6AB0-B74E-4B1D-90AD-F71615A5E6CE}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{69CDFB20-E47F-4E80-83C9-1B1B49D34894}"/>
   </bookViews>
   <sheets>
     <sheet name="LSEG.L News Data" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -78,79 +78,67 @@
     <t>sourceCode</t>
   </si>
   <si>
-    <t>Friday's Preview: Can London Stock Exchange Group rebound after being down?</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20250214:nNRAvf0ije:0</t>
-  </si>
-  <si>
-    <t>NS:GLOSTO</t>
-  </si>
-  <si>
-    <t>Can London Stock Exchange rebound after recent dip?</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20250214:nNRAvf0dpt:0</t>
+    <t>London Stock Exchange adds 7% in past 3 months</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20250219:nNRAvh4s9x:0</t>
   </si>
   <si>
     <t>NS:GLOROU</t>
   </si>
   <si>
-    <t>Eutelsat Communications SA - Eutelsat Communications: Second Quarter and First Half 2024-25 Results</t>
-  </si>
-  <si>
-    <t>urn:newsml:reuters.com:20250214:nNDL9RpMVp:1</t>
+    <t>Past Week: London Stock Exchange Group (LSEG: GBX11,705.0) down 3.2% in 2 weeks; -GBX390 [-3.2%]</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20250219:nNRAvh4r8b:0</t>
+  </si>
+  <si>
+    <t>NS:NEWMAR</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20250219:nNRAvh4rs9:0</t>
+  </si>
+  <si>
+    <t>London Stock Exchange Group (LSEG: GBX11,705.0) strengthens above moving average price; +GBX15 [+0.1%] Vol Index 1.2 [1 is avg]</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20250219:nNRAvh4pmn:0</t>
+  </si>
+  <si>
+    <t>Wednesday's Preview: Can London Stock Exchange continue its recent gains?</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20250219:nNRAvh3052:0</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20250219:nNRAvh2j9x:0</t>
+  </si>
+  <si>
+    <t>Traders look to see if London Stock Exchange's recent rally will continue</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20250219:nNRAvh2edj:0</t>
+  </si>
+  <si>
+    <t>German trading: London Stock Exchange Group (LS4C: EUR141.0) drops 1.4% on slipping relative strength; -EUR2 [-1.4%]</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20250219:nNRAvh262u:0</t>
+  </si>
+  <si>
+    <t>NS:GERCOM</t>
+  </si>
+  <si>
+    <t>urn:newsml:newsroom:20250219:nNRAvh1rf1:0</t>
+  </si>
+  <si>
+    <t>LSEG - Sustainability Policy 210.0KB • PDF</t>
+  </si>
+  <si>
+    <t>urn:newsml:reuters.com:20250219:nNDL2MpB1y:1</t>
   </si>
   <si>
     <t>NS:PUBT</t>
-  </si>
-  <si>
-    <t>German trading: London Stock Exchange Group (LS4C: EUR142.0) decreases on average volume</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20250214:nNRAveyqa5:0</t>
-  </si>
-  <si>
-    <t>NS:GERCOM</t>
-  </si>
-  <si>
-    <t>London Stock Exchange gains 7% in past 3 months</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20250214:nNRAveyiha:0</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20250213:nNRAvewq3s:0</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20250213:nNRAvewre1:0</t>
-  </si>
-  <si>
-    <t>LSEG Expands Coverage of Tick History</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20250213:nNRAvewag2:0</t>
-  </si>
-  <si>
-    <t>NS:MARUSA</t>
-  </si>
-  <si>
-    <t>London Stock Exchange Group (LSEG: GBX11,655.0) decreases GBX80.0, 2 days' volume in a day</t>
-  </si>
-  <si>
-    <t>urn:newsml:newsroom:20250213:nNRAvew4he:0</t>
-  </si>
-  <si>
-    <t>NS:NEWMAR</t>
-  </si>
-  <si>
-    <t>DJ Top 3% Stock Tradeweb Markets Aiming For A Fresh High -- IBD</t>
-  </si>
-  <si>
-    <t>urn:newsml:reuters.com:20250213:nDjc7fHX2j:2</t>
-  </si>
-  <si>
-    <t>NS:DJCP</t>
   </si>
 </sst>
 </file>
@@ -258,7 +246,7 @@
         <xdr:cNvPr id="3" name="MyPlot">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4DBD2AF-1AB8-863B-5900-51DFC36803EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAF33C72-67F5-7CAD-D399-EFFE1FCD5B00}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -609,7 +597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F969712-E896-4C0A-98FB-CEC18AF5302C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB34DB2D-A7C7-4D6F-A9C2-21BBBEF6E9F7}">
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -694,46 +682,46 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -741,43 +729,43 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -786,10 +774,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D72CA6F-7E1B-40C3-97FA-9F0C22605176}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86489108-D1C7-4ABE-98DD-838F517E6775}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0"/>
+    <sheetView topLeftCell="A21" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1613,7 +1601,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>